<commit_message>
Latest Automation testing file Changes
</commit_message>
<xml_diff>
--- a/SwarmHRAutomationProject/src/test/resources/excel/testdata.xlsx
+++ b/SwarmHRAutomationProject/src/test/resources/excel/testdata.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse-WorkSpace\SwarmHRAutomation\SwarmHRAutomationProject\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navee\git\swarmhrnextgenautomation\SwarmHRAutomationProject\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5EB5C2-09C9-4D48-AEB0-F61FFC1ABF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{649BA9E6-39B1-44CD-A43C-831BD81F182C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14676" windowHeight="5256"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="MyInfo" sheetId="2" r:id="rId2"/>
     <sheet name="test_suite" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -48,24 +47,12 @@
     <t>Y</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>mobile</t>
   </si>
   <si>
     <t>123-123-1221</t>
   </si>
   <si>
-    <t>naveen.dumbala@swarmhr.com</t>
-  </si>
-  <si>
-    <t>mvincses_occi</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
@@ -79,12 +66,18 @@
   </si>
   <si>
     <t>MyInfo</t>
+  </si>
+  <si>
+    <t>swarmadmin_spx</t>
+  </si>
+  <si>
+    <t>$w@rm@dmin_spx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,10 +116,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,21 +433,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA64A46-DF2A-4D25-9016-8D6B596DDEF0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,17 +455,54 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -482,79 +511,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED576651-8942-44C7-8E05-ACEDD8C6CA37}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B44FA1E2-CD44-4F84-AA96-B859AA801B0B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F910FA-A158-4B83-8B6B-42D142825B6B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>

</xml_diff>